<commit_message>
Transformaciones Finales a datos
</commit_message>
<xml_diff>
--- a/Modelos/Calculos_Modelos.xlsx
+++ b/Modelos/Calculos_Modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGM\Documents\Habi\Prueba Data Science\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30F0C7C-4A85-44C1-9BC1-2D2A950A577A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696C0E4E-56BE-408D-87FA-FCEBAB5D5C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="2" xr2:uid="{D278BB23-159C-48A0-BB88-7B063591FAE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{D278BB23-159C-48A0-BB88-7B063591FAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="precio_m2" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="15">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -1457,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61C1141-EF1C-487F-98B2-83336C35D258}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,9 +1469,11 @@
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1502,8 +1504,38 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1534,6 +1566,134 @@
       <c r="J2">
         <v>15</v>
       </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>0.1</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1">
+        <v>91837620.141484603</v>
+      </c>
+      <c r="T2">
+        <v>0.17870844335130001</v>
+      </c>
+      <c r="U2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1">
+        <v>92202532.692044497</v>
+      </c>
+      <c r="I3">
+        <v>0.18619268867327099</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>93065842.771723807</v>
+      </c>
+      <c r="I4">
+        <v>0.189967700342627</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>85558007.302483395</v>
+      </c>
+      <c r="I5">
+        <v>0.155435134275934</v>
+      </c>
+      <c r="J5">
+        <v>23</v>
+      </c>
+      <c r="S5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>